<commit_message>
Update the excel example
</commit_message>
<xml_diff>
--- a/Excel动手实验室 - 材料/00 - 操作介绍.xlsx
+++ b/Excel动手实验室 - 材料/00 - 操作介绍.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\OfficeTraining\Excel动手实验室 - 材料\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14460" windowHeight="5055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14460" windowHeight="5051"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="37">
   <si>
     <t>工作项目</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -183,13 +178,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -197,14 +192,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -213,7 +208,15 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -263,25 +266,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1">
@@ -293,50 +294,57 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Accent5" xfId="1" builtinId="45"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="强调文字颜色 5" xfId="1" builtinId="45"/>
+    <cellStyle name="百分比" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
     <dxf>
-      <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -352,17 +360,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="C5:J18" totalsRowCount="1">
-  <autoFilter ref="C5:J17"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="C5:I18" totalsRowCount="1">
+  <autoFilter ref="C5:I17"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="工作项目" totalsRowLabel="总计"/>
-    <tableColumn id="2" name="估计材料" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="估计材料" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="3" name="承包商"/>
-    <tableColumn id="4" name="截止时间"/>
     <tableColumn id="5" name="联系人"/>
-    <tableColumn id="6" name="投标" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="1"/>
-    <tableColumn id="7" name="实际成本" dataDxfId="10" totalsRowDxfId="0"/>
-    <tableColumn id="8" name="高于/低于预算"/>
+    <tableColumn id="6" name="投标" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="7" name="实际成本" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="4" name="截止时间" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -373,13 +380,13 @@
   <autoFilter ref="C5:J17"/>
   <tableColumns count="8">
     <tableColumn id="1" name="工作项目" totalsRowLabel="总计"/>
-    <tableColumn id="2" name="估计材料" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="5"/>
+    <tableColumn id="2" name="估计材料" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5"/>
     <tableColumn id="3" name="承包商"/>
     <tableColumn id="4" name="截止时间"/>
     <tableColumn id="5" name="联系人"/>
-    <tableColumn id="6" name="投标" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="4"/>
-    <tableColumn id="7" name="实际成本" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="3"/>
-    <tableColumn id="8" name="高于/低于预算" dataDxfId="6"/>
+    <tableColumn id="6" name="投标" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="7" name="实际成本" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="8" name="高于/低于预算" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -428,7 +435,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -463,7 +470,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -640,7 +647,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -654,7 +661,7 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -669,7 +676,7 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
     <col min="3" max="3" width="9" customWidth="1"/>
   </cols>
@@ -770,24 +777,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:J18"/>
+  <dimension ref="C5:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:10">
+    <row r="5" spans="3:9">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -798,22 +804,19 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10">
+    </row>
+    <row r="6" spans="3:9">
       <c r="C6" t="s">
         <v>2</v>
       </c>
@@ -823,20 +826,20 @@
       <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1">
+        <v>23000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>21500</v>
+      </c>
+      <c r="I6" s="2">
         <v>42079</v>
       </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="1">
-        <v>23000</v>
-      </c>
-      <c r="I6" s="1">
-        <v>21500</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10">
+    </row>
+    <row r="7" spans="3:9">
       <c r="C7" t="s">
         <v>3</v>
       </c>
@@ -846,20 +849,20 @@
       <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="1">
+        <v>85000</v>
+      </c>
+      <c r="H7" s="1">
+        <v>84923.31</v>
+      </c>
+      <c r="I7" s="2">
         <v>42105</v>
       </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="1">
-        <v>85000</v>
-      </c>
-      <c r="I7" s="1">
-        <v>84923.31</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10">
+    </row>
+    <row r="8" spans="3:9">
       <c r="C8" t="s">
         <v>4</v>
       </c>
@@ -869,20 +872,20 @@
       <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1">
+        <v>15000</v>
+      </c>
+      <c r="H8" s="1">
+        <v>14630</v>
+      </c>
+      <c r="I8" s="2">
         <v>42105</v>
       </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="1">
-        <v>15000</v>
-      </c>
-      <c r="I8" s="1">
-        <v>14630</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10">
+    </row>
+    <row r="9" spans="3:9">
       <c r="C9" t="s">
         <v>5</v>
       </c>
@@ -892,20 +895,20 @@
       <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H9" s="1">
+        <v>8090</v>
+      </c>
+      <c r="I9" s="2">
         <v>42107</v>
       </c>
-      <c r="G9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="1">
-        <v>10000</v>
-      </c>
-      <c r="I9" s="1">
-        <v>8090</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10">
+    </row>
+    <row r="10" spans="3:9">
       <c r="C10" t="s">
         <v>6</v>
       </c>
@@ -915,20 +918,20 @@
       <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4800</v>
+      </c>
+      <c r="H10" s="1">
+        <v>4890</v>
+      </c>
+      <c r="I10" s="2">
         <v>42099</v>
       </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="1">
-        <v>4800</v>
-      </c>
-      <c r="I10" s="1">
-        <v>4890</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10">
+    </row>
+    <row r="11" spans="3:9">
       <c r="C11" t="s">
         <v>7</v>
       </c>
@@ -938,20 +941,20 @@
       <c r="E11" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="1">
+        <v>57800</v>
+      </c>
+      <c r="H11" s="1">
+        <v>56200</v>
+      </c>
+      <c r="I11" s="2">
         <v>42072</v>
       </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="1">
-        <v>57800</v>
-      </c>
-      <c r="I11" s="1">
-        <v>56200</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10">
+    </row>
+    <row r="12" spans="3:9">
       <c r="C12" t="s">
         <v>8</v>
       </c>
@@ -961,20 +964,20 @@
       <c r="E12" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="1">
+        <v>15870</v>
+      </c>
+      <c r="H12" s="1">
+        <v>7080</v>
+      </c>
+      <c r="I12" s="2">
         <v>42081</v>
       </c>
-      <c r="G12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="1">
-        <v>15870</v>
-      </c>
-      <c r="I12" s="1">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10">
+    </row>
+    <row r="13" spans="3:9">
       <c r="C13" t="s">
         <v>9</v>
       </c>
@@ -984,20 +987,20 @@
       <c r="E13" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="1">
+        <v>8870</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4120</v>
+      </c>
+      <c r="I13" s="2">
         <v>42086</v>
       </c>
-      <c r="G13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="1">
-        <v>8870</v>
-      </c>
-      <c r="I13" s="1">
-        <v>4120</v>
-      </c>
-    </row>
-    <row r="14" spans="3:10">
+    </row>
+    <row r="14" spans="3:9">
       <c r="C14" t="s">
         <v>10</v>
       </c>
@@ -1007,20 +1010,20 @@
       <c r="E14" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3790</v>
+      </c>
+      <c r="H14" s="1">
+        <v>41500</v>
+      </c>
+      <c r="I14" s="2">
         <v>42079</v>
       </c>
-      <c r="G14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="1">
-        <v>3790</v>
-      </c>
-      <c r="I14" s="1">
-        <v>41500</v>
-      </c>
-    </row>
-    <row r="15" spans="3:10">
+    </row>
+    <row r="15" spans="3:9">
       <c r="C15" t="s">
         <v>11</v>
       </c>
@@ -1030,20 +1033,20 @@
       <c r="E15" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="1">
+        <v>41000</v>
+      </c>
+      <c r="H15" s="1">
+        <v>14530</v>
+      </c>
+      <c r="I15" s="2">
         <v>42114</v>
       </c>
-      <c r="G15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="1">
-        <v>41000</v>
-      </c>
-      <c r="I15" s="1">
-        <v>14530</v>
-      </c>
-    </row>
-    <row r="16" spans="3:10">
+    </row>
+    <row r="16" spans="3:9">
       <c r="C16" t="s">
         <v>18</v>
       </c>
@@ -1053,17 +1056,17 @@
       <c r="E16" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20000</v>
+      </c>
+      <c r="H16" s="1">
+        <v>18750</v>
+      </c>
+      <c r="I16" s="2">
         <v>42114</v>
-      </c>
-      <c r="G16" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="1">
-        <v>20000</v>
-      </c>
-      <c r="I16" s="1">
-        <v>18750</v>
       </c>
     </row>
     <row r="17" spans="3:9">
@@ -1076,17 +1079,17 @@
       <c r="E17" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="1">
+        <v>5000</v>
+      </c>
+      <c r="H17" s="1">
+        <v>4250</v>
+      </c>
+      <c r="I17" s="2">
         <v>42093</v>
-      </c>
-      <c r="G17" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="1">
-        <v>5000</v>
-      </c>
-      <c r="I17" s="1">
-        <v>4250</v>
       </c>
     </row>
     <row r="18" spans="3:9">
@@ -1097,11 +1100,11 @@
         <f>SUBTOTAL(109,Table3[估计材料])</f>
         <v>289950</v>
       </c>
-      <c r="H18" s="1">
+      <c r="G18" s="1">
         <f>SUBTOTAL(109,Table3[投标])</f>
         <v>290130</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1120,15 +1123,15 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:10">
@@ -1473,31 +1476,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:G20"/>
+  <dimension ref="C5:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:7">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1633,21 +1636,17 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="18" spans="3:5">
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5">
-      <c r="C20" t="s">
+    <row r="19" spans="3:5">
+      <c r="C19" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D19" s="6">
         <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>